<commit_message>
Updated to version 2 data and renamed CONT into FOOD
</commit_message>
<xml_diff>
--- a/Mappings/Reporting_template_AGMIP_Jan2017_v3.xlsx
+++ b/Mappings/Reporting_template_AGMIP_Jan2017_v3.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\AgriCLIM50_2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10656" windowHeight="8352" tabRatio="754" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10650" windowHeight="8355" tabRatio="754"/>
   </bookViews>
   <sheets>
     <sheet name="Listing_template" sheetId="8" r:id="rId1"/>
@@ -32,7 +27,7 @@
     <author>Hugo Valin</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="1" shapeId="0">
+    <comment ref="G3" authorId="1">
       <text>
         <r>
           <rPr>
@@ -3218,7 +3213,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3608,7 +3603,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3643,7 +3638,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3854,18 +3849,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="11.44140625" style="13"/>
+    <col min="1" max="6" width="11.42578125" style="13"/>
     <col min="7" max="7" width="16" style="13" customWidth="1"/>
-    <col min="8" max="9" width="11.44140625" style="13"/>
-    <col min="10" max="10" width="54.33203125" style="13" customWidth="1"/>
-    <col min="11" max="16384" width="11.44140625" style="13"/>
+    <col min="8" max="9" width="11.42578125" style="13"/>
+    <col min="10" max="10" width="54.28515625" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3891,7 +3886,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>190</v>
       </c>
@@ -3917,7 +3912,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="56"/>
       <c r="B3" s="56"/>
       <c r="C3" s="44" t="s">
@@ -3939,7 +3934,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="56"/>
       <c r="B4" s="56"/>
       <c r="C4" s="44" t="s">
@@ -3961,7 +3956,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="56"/>
       <c r="B5" s="56"/>
       <c r="C5" s="44" t="s">
@@ -3983,7 +3978,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="56"/>
       <c r="B6" s="56"/>
       <c r="C6" s="44" t="s">
@@ -4002,7 +3997,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="56"/>
       <c r="B7" s="56"/>
       <c r="C7" s="44" t="s">
@@ -4021,7 +4016,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="56"/>
       <c r="B8" s="56"/>
       <c r="C8" s="44" t="s">
@@ -4040,7 +4035,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="56"/>
       <c r="B9" s="56"/>
       <c r="C9" s="44" t="s">
@@ -4059,7 +4054,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="56"/>
       <c r="B10" s="56"/>
       <c r="C10" s="44" t="s">
@@ -4078,7 +4073,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="56"/>
       <c r="B11" s="56"/>
       <c r="C11" s="44" t="s">
@@ -4094,7 +4089,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C12" s="44" t="s">
         <v>60</v>
       </c>
@@ -4108,7 +4103,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C13" s="44" t="s">
         <v>172</v>
       </c>
@@ -4122,7 +4117,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C14" s="44" t="s">
         <v>175</v>
       </c>
@@ -4137,7 +4132,7 @@
       </c>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C15" s="44" t="s">
         <v>22</v>
       </c>
@@ -4152,7 +4147,7 @@
       </c>
       <c r="H15" s="58"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C16" s="44" t="s">
         <v>180</v>
       </c>
@@ -4167,7 +4162,7 @@
       </c>
       <c r="H16" s="58"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" s="44" t="s">
         <v>184</v>
       </c>
@@ -4182,7 +4177,7 @@
       </c>
       <c r="H17" s="58"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C18" s="44" t="s">
         <v>187</v>
       </c>
@@ -4197,7 +4192,7 @@
       </c>
       <c r="H18" s="58"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C19" s="44" t="s">
         <v>58</v>
       </c>
@@ -4211,7 +4206,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C20" s="37" t="s">
         <v>970</v>
       </c>
@@ -4222,7 +4217,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D21" s="47" t="s">
         <v>96</v>
       </c>
@@ -4230,7 +4225,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C22" s="46"/>
       <c r="D22" s="47" t="s">
         <v>97</v>
@@ -4239,7 +4234,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D23" s="49" t="s">
         <v>75</v>
       </c>
@@ -4247,7 +4242,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D24" s="47" t="s">
         <v>127</v>
       </c>
@@ -4255,7 +4250,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D25" s="47" t="s">
         <v>76</v>
       </c>
@@ -4263,7 +4258,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D26" s="44" t="s">
         <v>77</v>
       </c>
@@ -4271,7 +4266,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D27" s="44" t="s">
         <v>78</v>
       </c>
@@ -4279,7 +4274,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D28" s="67" t="s">
         <v>1005</v>
       </c>
@@ -4287,7 +4282,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D29" s="67" t="s">
         <v>1006</v>
       </c>
@@ -4295,7 +4290,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D30" s="67" t="s">
         <v>988</v>
       </c>
@@ -4303,7 +4298,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D31" s="67" t="s">
         <v>1008</v>
       </c>
@@ -4311,7 +4306,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D32" s="37" t="s">
         <v>104</v>
       </c>
@@ -4319,7 +4314,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D33" s="37" t="s">
         <v>103</v>
       </c>
@@ -4327,7 +4322,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D34" s="37" t="s">
         <v>102</v>
       </c>
@@ -4335,7 +4330,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D35" s="37" t="s">
         <v>34</v>
       </c>
@@ -4343,17 +4338,17 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E36" s="40" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E37" s="40" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E38" s="62" t="s">
         <v>1045</v>
       </c>
@@ -4369,23 +4364,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="13" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="13"/>
+    <col min="1" max="1" width="8.85546875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="43"/>
       <c r="B3" s="43" t="s">
         <v>24</v>
@@ -4397,7 +4392,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B4" s="44" t="s">
         <v>88</v>
       </c>
@@ -4408,7 +4403,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B5" s="44" t="s">
         <v>16</v>
       </c>
@@ -4419,7 +4414,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B6" s="44" t="s">
         <v>94</v>
       </c>
@@ -4430,7 +4425,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B7" s="44" t="s">
         <v>90</v>
       </c>
@@ -4441,7 +4436,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8" s="44" t="s">
         <v>89</v>
       </c>
@@ -4452,7 +4447,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B9" s="37" t="s">
         <v>45</v>
       </c>
@@ -4463,7 +4458,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B10" s="72" t="s">
         <v>53</v>
       </c>
@@ -4474,7 +4469,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B11" s="37" t="s">
         <v>95</v>
       </c>
@@ -4485,7 +4480,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="44" t="s">
         <v>91</v>
       </c>
@@ -4496,7 +4491,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="44" t="s">
         <v>92</v>
       </c>
@@ -4507,7 +4502,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B14" s="44" t="s">
         <v>93</v>
       </c>
@@ -4518,7 +4513,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" s="37" t="s">
         <v>1030</v>
       </c>
@@ -4529,7 +4524,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B16" s="37" t="s">
         <v>104</v>
       </c>
@@ -4537,7 +4532,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B17" s="37" t="s">
         <v>127</v>
       </c>
@@ -4545,7 +4540,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="46"/>
       <c r="B18" s="47" t="s">
         <v>96</v>
@@ -4557,7 +4552,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="46"/>
       <c r="B19" s="47" t="s">
         <v>97</v>
@@ -4569,7 +4564,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="46"/>
       <c r="B20" s="47" t="s">
         <v>102</v>
@@ -4579,7 +4574,7 @@
       </c>
       <c r="D20" s="46"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="48" t="s">
         <v>997</v>
       </c>
@@ -4587,7 +4582,7 @@
       <c r="C21" s="46"/>
       <c r="D21" s="46"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="48"/>
       <c r="B22" s="67" t="s">
         <v>987</v>
@@ -4597,7 +4592,7 @@
       </c>
       <c r="D22" s="46"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="48"/>
       <c r="B23" s="67" t="s">
         <v>1018</v>
@@ -4607,7 +4602,7 @@
       </c>
       <c r="D23" s="46"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="48"/>
       <c r="B24" s="67" t="s">
         <v>989</v>
@@ -4617,7 +4612,7 @@
       </c>
       <c r="D24" s="46"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="46"/>
       <c r="B25" s="67" t="s">
         <v>458</v>
@@ -4627,7 +4622,7 @@
       </c>
       <c r="D25" s="46"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="46"/>
       <c r="B26" s="67" t="s">
         <v>981</v>
@@ -4637,7 +4632,7 @@
       </c>
       <c r="D26" s="46"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="46"/>
       <c r="B27" s="67" t="s">
         <v>983</v>
@@ -4647,7 +4642,7 @@
       </c>
       <c r="D27" s="46"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="46"/>
       <c r="B28" s="67" t="s">
         <v>985</v>
@@ -4657,7 +4652,7 @@
       </c>
       <c r="D28" s="46"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="48" t="s">
         <v>100</v>
       </c>
@@ -4665,7 +4660,7 @@
       <c r="C29" s="46"/>
       <c r="D29" s="46"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="46"/>
       <c r="B30" s="49" t="s">
         <v>75</v>
@@ -4677,7 +4672,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="46"/>
       <c r="B31" s="47" t="s">
         <v>76</v>
@@ -4689,7 +4684,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="46"/>
       <c r="B32" s="49" t="s">
         <v>77</v>
@@ -4701,7 +4696,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="29"/>
       <c r="B33" s="51" t="s">
         <v>78</v>
@@ -4711,17 +4706,17 @@
       </c>
       <c r="D33" s="53"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D34" s="54"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>101</v>
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="25"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B36" s="44" t="s">
         <v>75</v>
       </c>
@@ -4729,7 +4724,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B37" s="37" t="s">
         <v>104</v>
       </c>
@@ -4738,7 +4733,7 @@
       </c>
       <c r="D37" s="25"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B38" s="37" t="s">
         <v>103</v>
       </c>
@@ -4747,7 +4742,7 @@
       </c>
       <c r="D38" s="25"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B39" s="37" t="s">
         <v>97</v>
       </c>
@@ -4756,7 +4751,7 @@
       </c>
       <c r="D39" s="25"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" s="37" t="s">
         <v>34</v>
       </c>
@@ -4765,12 +4760,12 @@
       </c>
       <c r="D40" s="25"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>996</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B42" s="44" t="s">
         <v>77</v>
       </c>
@@ -4778,7 +4773,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B43" s="37" t="s">
         <v>102</v>
       </c>
@@ -4786,12 +4781,12 @@
         <v>995</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" s="77" t="s">
         <v>1042</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B45" s="87" t="s">
         <v>1005</v>
       </c>
@@ -4800,7 +4795,7 @@
       </c>
       <c r="E45" s="25"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B46" s="87" t="s">
         <v>1006</v>
       </c>
@@ -4809,7 +4804,7 @@
       </c>
       <c r="E46" s="25"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B47" s="87" t="s">
         <v>988</v>
       </c>
@@ -4818,7 +4813,7 @@
       </c>
       <c r="E47" s="25"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B48" s="87" t="s">
         <v>1008</v>
       </c>
@@ -4843,20 +4838,20 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="25"/>
-    <col min="2" max="2" width="33.6640625" style="25" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" style="25" customWidth="1"/>
-    <col min="4" max="10" width="6.6640625" style="25" customWidth="1"/>
-    <col min="11" max="11" width="6.6640625" style="78" customWidth="1"/>
-    <col min="12" max="16" width="6.6640625" style="25" customWidth="1"/>
-    <col min="17" max="17" width="6.6640625" style="78" customWidth="1"/>
-    <col min="18" max="26" width="6.6640625" style="25" customWidth="1"/>
-    <col min="27" max="16384" width="9.109375" style="25"/>
+    <col min="1" max="1" width="9.140625" style="25"/>
+    <col min="2" max="2" width="33.7109375" style="25" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="25" customWidth="1"/>
+    <col min="4" max="10" width="6.7109375" style="25" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" style="78" customWidth="1"/>
+    <col min="12" max="16" width="6.7109375" style="25" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" style="78" customWidth="1"/>
+    <col min="18" max="26" width="6.7109375" style="25" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -4974,7 +4969,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="29"/>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
@@ -5060,7 +5055,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>65</v>
       </c>
@@ -5095,7 +5090,7 @@
       <c r="X4" s="34"/>
       <c r="Y4" s="34"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>66</v>
       </c>
@@ -5130,7 +5125,7 @@
       <c r="X5" s="34"/>
       <c r="Y5" s="34"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
@@ -5209,7 +5204,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>4</v>
       </c>
@@ -5276,7 +5271,7 @@
       <c r="X7" s="34"/>
       <c r="Y7" s="34"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
@@ -5341,7 +5336,7 @@
       <c r="X8" s="34"/>
       <c r="Y8" s="34"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="60" t="s">
         <v>1013</v>
       </c>
@@ -5399,7 +5394,7 @@
       <c r="AC9" s="60"/>
       <c r="AD9" s="60"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="60" t="s">
         <v>1012</v>
       </c>
@@ -5457,7 +5452,7 @@
       <c r="AC10" s="60"/>
       <c r="AD10" s="60"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
         <v>62</v>
       </c>
@@ -5511,7 +5506,7 @@
       <c r="AC11" s="82"/>
       <c r="AD11" s="82"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>15</v>
       </c>
@@ -5570,7 +5565,7 @@
       <c r="AC12" s="78"/>
       <c r="AD12" s="78"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="60" t="s">
         <v>1014</v>
       </c>
@@ -5628,7 +5623,7 @@
       <c r="AC13" s="60"/>
       <c r="AD13" s="60"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="60" t="s">
         <v>1015</v>
       </c>
@@ -5686,7 +5681,7 @@
       <c r="AC14" s="60"/>
       <c r="AD14" s="60"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
         <v>67</v>
       </c>
@@ -5745,7 +5740,7 @@
       <c r="AC15" s="78"/>
       <c r="AD15" s="78"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="62" t="s">
         <v>998</v>
       </c>
@@ -5805,7 +5800,7 @@
       <c r="AC16" s="60"/>
       <c r="AD16" s="60"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
         <v>63</v>
       </c>
@@ -5849,7 +5844,7 @@
       <c r="AC17" s="37"/>
       <c r="AD17" s="37"/>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
         <v>68</v>
       </c>
@@ -5893,7 +5888,7 @@
       <c r="AC18" s="37"/>
       <c r="AD18" s="37"/>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="s">
         <v>106</v>
       </c>
@@ -5941,7 +5936,7 @@
       <c r="AC19" s="37"/>
       <c r="AD19" s="37"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="40" t="s">
         <v>105</v>
       </c>
@@ -5989,7 +5984,7 @@
       <c r="AC20" s="37"/>
       <c r="AD20" s="37"/>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>9</v>
       </c>
@@ -6054,7 +6049,7 @@
       <c r="X21" s="34"/>
       <c r="Y21" s="34"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>10</v>
       </c>
@@ -6115,7 +6110,7 @@
       <c r="AC22" s="78"/>
       <c r="AD22" s="78"/>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
         <v>10</v>
       </c>
@@ -6177,7 +6172,7 @@
       <c r="AC23" s="37"/>
       <c r="AD23" s="37"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>11</v>
       </c>
@@ -6248,7 +6243,7 @@
       <c r="AC24" s="78"/>
       <c r="AD24" s="78"/>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>13</v>
       </c>
@@ -6319,7 +6314,7 @@
       <c r="AC25" s="78"/>
       <c r="AD25" s="78"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>12</v>
       </c>
@@ -6390,7 +6385,7 @@
       <c r="AC26" s="78"/>
       <c r="AD26" s="78"/>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="41" t="s">
         <v>70</v>
       </c>
@@ -6449,7 +6444,7 @@
       <c r="AC27" s="78"/>
       <c r="AD27" s="78"/>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
         <v>64</v>
       </c>
@@ -6506,7 +6501,7 @@
       <c r="AC28" s="78"/>
       <c r="AD28" s="78"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="41" t="s">
         <v>23</v>
       </c>
@@ -6575,7 +6570,7 @@
       <c r="AC29" s="78"/>
       <c r="AD29" s="78"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>7</v>
       </c>
@@ -6648,7 +6643,7 @@
       <c r="AC30" s="78"/>
       <c r="AD30" s="78"/>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
         <v>8</v>
       </c>
@@ -6719,7 +6714,7 @@
       <c r="AC31" s="78"/>
       <c r="AD31" s="78"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>14</v>
       </c>
@@ -6790,7 +6785,7 @@
       <c r="AC32" s="78"/>
       <c r="AD32" s="78"/>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="37" t="s">
         <v>286</v>
       </c>
@@ -6850,7 +6845,7 @@
       <c r="AC33" s="37"/>
       <c r="AD33" s="37"/>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="37" t="s">
         <v>286</v>
       </c>
@@ -6910,7 +6905,7 @@
       <c r="AC34" s="37"/>
       <c r="AD34" s="37"/>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="37" t="s">
         <v>287</v>
       </c>
@@ -6970,7 +6965,7 @@
       <c r="AC35" s="37"/>
       <c r="AD35" s="37"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="37" t="s">
         <v>287</v>
       </c>
@@ -7030,7 +7025,7 @@
       <c r="AC36" s="37"/>
       <c r="AD36" s="37"/>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="37" t="s">
         <v>288</v>
       </c>
@@ -7090,7 +7085,7 @@
       <c r="AC37" s="37"/>
       <c r="AD37" s="37"/>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="37" t="s">
         <v>288</v>
       </c>
@@ -7150,7 +7145,7 @@
       <c r="AC38" s="37"/>
       <c r="AD38" s="37"/>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="37" t="s">
         <v>289</v>
       </c>
@@ -7210,7 +7205,7 @@
       <c r="AC39" s="37"/>
       <c r="AD39" s="37"/>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="37" t="s">
         <v>289</v>
       </c>
@@ -7270,7 +7265,7 @@
       <c r="AC40" s="37"/>
       <c r="AD40" s="37"/>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="42" t="s">
         <v>107</v>
       </c>
@@ -7350,7 +7345,7 @@
       <c r="AC41" s="82"/>
       <c r="AD41" s="82"/>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="42" t="s">
         <v>108</v>
       </c>
@@ -7396,7 +7391,7 @@
       <c r="AC42" s="82"/>
       <c r="AD42" s="82"/>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="42" t="s">
         <v>109</v>
       </c>
@@ -7452,7 +7447,7 @@
       <c r="AC43" s="82"/>
       <c r="AD43" s="82"/>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" s="42" t="s">
         <v>110</v>
       </c>
@@ -7528,7 +7523,7 @@
       <c r="AC44" s="82"/>
       <c r="AD44" s="82"/>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45" s="88" t="s">
         <v>1045</v>
       </c>
@@ -7582,19 +7577,19 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="1" customWidth="1"/>
-    <col min="7" max="20" width="8.88671875" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.109375" style="1"/>
+    <col min="7" max="20" width="8.85546875" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -7608,7 +7603,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -7637,7 +7632,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -7664,7 +7659,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -7691,7 +7686,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -7718,7 +7713,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>155</v>
       </c>
@@ -7745,7 +7740,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>158</v>
       </c>
@@ -7772,7 +7767,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>59</v>
       </c>
@@ -7799,7 +7794,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>163</v>
       </c>
@@ -7826,7 +7821,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>166</v>
       </c>
@@ -7856,7 +7851,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -7886,7 +7881,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -7913,7 +7908,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>60</v>
       </c>
@@ -7941,7 +7936,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>172</v>
       </c>
@@ -7969,7 +7964,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>175</v>
       </c>
@@ -7997,7 +7992,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D16" s="2"/>
       <c r="E16"/>
       <c r="F16" s="6" t="s">
@@ -8016,7 +8011,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -8046,7 +8041,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>180</v>
       </c>
@@ -8076,7 +8071,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>184</v>
       </c>
@@ -8106,7 +8101,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>187</v>
       </c>
@@ -8136,7 +8131,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E21"/>
       <c r="F21" s="6" t="s">
         <v>363</v>
@@ -8154,7 +8149,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
@@ -8181,7 +8176,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E23"/>
       <c r="F23" s="6" t="s">
         <v>369</v>
@@ -8199,7 +8194,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>967</v>
       </c>
@@ -8220,7 +8215,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="68" t="s">
         <v>971</v>
       </c>
@@ -8247,7 +8242,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E26"/>
       <c r="F26" s="6" t="s">
         <v>378</v>
@@ -8265,7 +8260,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E27"/>
       <c r="F27" s="6" t="s">
         <v>381</v>
@@ -8283,7 +8278,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E28"/>
       <c r="F28" s="6" t="s">
         <v>384</v>
@@ -8301,7 +8296,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E29"/>
       <c r="F29" s="6" t="s">
         <v>27</v>
@@ -8319,7 +8314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E30"/>
       <c r="F30" s="6" t="s">
         <v>388</v>
@@ -8337,7 +8332,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E31"/>
       <c r="F31" s="6" t="s">
         <v>391</v>
@@ -8355,7 +8350,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E32"/>
       <c r="F32" s="6" t="s">
         <v>394</v>
@@ -8373,7 +8368,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E33"/>
       <c r="F33" s="6" t="s">
         <v>397</v>
@@ -8391,7 +8386,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E34"/>
       <c r="F34" s="6" t="s">
         <v>400</v>
@@ -8409,7 +8404,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E35"/>
       <c r="F35" s="6" t="s">
         <v>403</v>
@@ -8427,7 +8422,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E36"/>
       <c r="F36" s="6" t="s">
         <v>406</v>
@@ -8445,7 +8440,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="37" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E37"/>
       <c r="F37" s="6" t="s">
         <v>26</v>
@@ -8463,7 +8458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E38"/>
       <c r="F38" s="6" t="s">
         <v>410</v>
@@ -8481,7 +8476,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E39"/>
       <c r="F39" s="6" t="s">
         <v>413</v>
@@ -8499,7 +8494,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E40"/>
       <c r="F40" s="6" t="s">
         <v>416</v>
@@ -8517,7 +8512,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="41" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E41"/>
       <c r="F41" s="6" t="s">
         <v>419</v>
@@ -8535,7 +8530,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E42"/>
       <c r="F42" s="6" t="s">
         <v>422</v>
@@ -8553,7 +8548,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E43"/>
       <c r="F43" s="6" t="s">
         <v>28</v>
@@ -8571,7 +8566,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E44"/>
       <c r="F44" s="6" t="s">
         <v>426</v>
@@ -8589,7 +8584,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E45"/>
       <c r="F45" s="6" t="s">
         <v>429</v>
@@ -8607,7 +8602,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="46" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E46"/>
       <c r="F46" s="6" t="s">
         <v>432</v>
@@ -8625,7 +8620,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E47"/>
       <c r="F47" s="6" t="s">
         <v>435</v>
@@ -8643,7 +8638,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="48" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E48"/>
       <c r="F48" s="6" t="s">
         <v>438</v>
@@ -8661,7 +8656,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E49"/>
       <c r="F49" s="6" t="s">
         <v>441</v>
@@ -8679,7 +8674,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="50" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E50"/>
       <c r="F50" s="6" t="s">
         <v>444</v>
@@ -8697,7 +8692,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E51"/>
       <c r="F51" s="6" t="s">
         <v>447</v>
@@ -8715,7 +8710,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="52" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E52"/>
       <c r="F52" s="6" t="s">
         <v>450</v>
@@ -8733,7 +8728,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E53"/>
       <c r="F53" s="6" t="s">
         <v>453</v>
@@ -8751,7 +8746,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E54"/>
       <c r="F54" s="6" t="s">
         <v>456</v>
@@ -8769,7 +8764,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E55"/>
       <c r="F55" s="6" t="s">
         <v>459</v>
@@ -8787,7 +8782,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="56" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E56"/>
       <c r="F56" s="6" t="s">
         <v>462</v>
@@ -8805,7 +8800,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E57"/>
       <c r="F57" s="6" t="s">
         <v>465</v>
@@ -8823,7 +8818,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="58" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E58"/>
       <c r="F58" s="6" t="s">
         <v>468</v>
@@ -8841,7 +8836,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="59" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E59"/>
       <c r="F59" s="6" t="s">
         <v>471</v>
@@ -8859,7 +8854,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E60"/>
       <c r="F60" s="6" t="s">
         <v>474</v>
@@ -8877,7 +8872,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="61" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E61"/>
       <c r="F61" s="6" t="s">
         <v>477</v>
@@ -8895,7 +8890,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="62" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E62"/>
       <c r="F62" s="6" t="s">
         <v>480</v>
@@ -8913,7 +8908,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="63" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E63"/>
       <c r="F63" s="6" t="s">
         <v>483</v>
@@ -8931,7 +8926,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="64" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E64"/>
       <c r="F64" s="6" t="s">
         <v>486</v>
@@ -8949,7 +8944,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E65"/>
       <c r="F65" s="6" t="s">
         <v>489</v>
@@ -8967,7 +8962,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E66"/>
       <c r="F66" s="6" t="s">
         <v>492</v>
@@ -8985,7 +8980,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="67" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E67"/>
       <c r="F67" s="6" t="s">
         <v>495</v>
@@ -9003,7 +8998,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="68" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E68"/>
       <c r="F68" s="6" t="s">
         <v>498</v>
@@ -9021,7 +9016,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="69" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E69"/>
       <c r="F69" s="6" t="s">
         <v>501</v>
@@ -9039,7 +9034,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E70"/>
       <c r="F70" s="6" t="s">
         <v>504</v>
@@ -9057,7 +9052,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="71" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E71"/>
       <c r="F71" s="6" t="s">
         <v>507</v>
@@ -9075,7 +9070,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="72" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E72"/>
       <c r="F72" s="6" t="s">
         <v>510</v>
@@ -9093,7 +9088,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="73" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E73"/>
       <c r="F73" s="6" t="s">
         <v>513</v>
@@ -9111,7 +9106,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="74" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E74"/>
       <c r="F74" s="6" t="s">
         <v>516</v>
@@ -9129,7 +9124,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="75" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E75"/>
       <c r="F75" s="6" t="s">
         <v>519</v>
@@ -9147,7 +9142,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E76"/>
       <c r="F76" s="6" t="s">
         <v>522</v>
@@ -9165,7 +9160,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="77" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E77"/>
       <c r="F77" s="6" t="s">
         <v>525</v>
@@ -9183,7 +9178,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E78"/>
       <c r="F78" s="6" t="s">
         <v>528</v>
@@ -9201,7 +9196,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E79"/>
       <c r="F79" s="6" t="s">
         <v>531</v>
@@ -9219,7 +9214,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="80" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E80"/>
       <c r="F80" s="6" t="s">
         <v>534</v>
@@ -9237,7 +9232,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="81" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E81"/>
       <c r="F81" s="6" t="s">
         <v>537</v>
@@ -9255,7 +9250,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="82" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E82"/>
       <c r="F82" s="6" t="s">
         <v>540</v>
@@ -9273,7 +9268,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="83" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E83"/>
       <c r="F83" s="6" t="s">
         <v>543</v>
@@ -9291,7 +9286,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="84" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E84"/>
       <c r="F84" s="6" t="s">
         <v>546</v>
@@ -9309,7 +9304,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="85" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E85"/>
       <c r="F85" s="6" t="s">
         <v>549</v>
@@ -9327,7 +9322,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="86" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E86"/>
       <c r="F86" s="6" t="s">
         <v>552</v>
@@ -9345,7 +9340,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="87" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E87"/>
       <c r="F87" s="6" t="s">
         <v>555</v>
@@ -9363,7 +9358,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="88" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E88"/>
       <c r="F88" s="6" t="s">
         <v>558</v>
@@ -9381,7 +9376,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E89"/>
       <c r="F89" s="6" t="s">
         <v>561</v>
@@ -9399,7 +9394,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="90" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E90"/>
       <c r="F90" s="6" t="s">
         <v>564</v>
@@ -9417,7 +9412,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="91" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E91"/>
       <c r="F91" s="6" t="s">
         <v>29</v>
@@ -9435,7 +9430,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E92"/>
       <c r="F92" s="6" t="s">
         <v>568</v>
@@ -9453,7 +9448,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E93"/>
       <c r="F93" s="6" t="s">
         <v>571</v>
@@ -9471,7 +9466,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="94" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E94"/>
       <c r="F94" s="6" t="s">
         <v>574</v>
@@ -9489,7 +9484,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="95" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E95"/>
       <c r="F95" s="6" t="s">
         <v>577</v>
@@ -9507,7 +9502,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="96" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E96"/>
       <c r="F96" s="6" t="s">
         <v>580</v>
@@ -9525,7 +9520,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="97" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E97"/>
       <c r="F97" s="6" t="s">
         <v>583</v>
@@ -9543,7 +9538,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="98" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E98"/>
       <c r="F98" s="6" t="s">
         <v>586</v>
@@ -9561,7 +9556,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="99" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E99"/>
       <c r="F99" s="6" t="s">
         <v>589</v>
@@ -9579,7 +9574,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E100"/>
       <c r="F100" s="6" t="s">
         <v>592</v>
@@ -9597,7 +9592,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="101" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E101"/>
       <c r="F101" s="6" t="s">
         <v>595</v>
@@ -9615,7 +9610,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="102" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E102"/>
       <c r="F102" s="6" t="s">
         <v>598</v>
@@ -9633,7 +9628,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="103" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E103"/>
       <c r="F103" s="6" t="s">
         <v>601</v>
@@ -9651,7 +9646,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="104" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E104"/>
       <c r="F104" s="6" t="s">
         <v>604</v>
@@ -9669,7 +9664,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="105" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E105"/>
       <c r="F105" s="6" t="s">
         <v>607</v>
@@ -9687,7 +9682,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="106" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E106"/>
       <c r="F106" s="6" t="s">
         <v>610</v>
@@ -9705,7 +9700,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="107" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E107"/>
       <c r="F107" s="6" t="s">
         <v>613</v>
@@ -9723,7 +9718,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="108" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E108"/>
       <c r="F108" s="6" t="s">
         <v>616</v>
@@ -9741,7 +9736,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="109" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E109"/>
       <c r="F109" s="6" t="s">
         <v>619</v>
@@ -9759,7 +9754,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="110" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E110"/>
       <c r="F110" s="6" t="s">
         <v>622</v>
@@ -9777,7 +9772,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="111" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E111"/>
       <c r="F111" s="6" t="s">
         <v>625</v>
@@ -9795,7 +9790,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="112" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E112"/>
       <c r="F112" s="6" t="s">
         <v>628</v>
@@ -9813,7 +9808,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="113" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E113"/>
       <c r="F113" s="6" t="s">
         <v>631</v>
@@ -9831,7 +9826,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="114" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E114"/>
       <c r="F114" s="6" t="s">
         <v>634</v>
@@ -9849,7 +9844,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="115" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E115"/>
       <c r="F115" s="6" t="s">
         <v>637</v>
@@ -9867,7 +9862,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E116"/>
       <c r="F116" s="6" t="s">
         <v>640</v>
@@ -9885,7 +9880,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="117" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E117"/>
       <c r="F117" s="6" t="s">
         <v>643</v>
@@ -9903,7 +9898,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="118" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E118"/>
       <c r="F118" s="6" t="s">
         <v>646</v>
@@ -9921,7 +9916,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="119" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E119"/>
       <c r="F119" s="6" t="s">
         <v>649</v>
@@ -9939,7 +9934,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="120" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E120"/>
       <c r="F120" s="6" t="s">
         <v>652</v>
@@ -9957,7 +9952,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="121" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E121"/>
       <c r="F121" s="6" t="s">
         <v>655</v>
@@ -9975,7 +9970,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="122" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E122"/>
       <c r="F122" s="6" t="s">
         <v>658</v>
@@ -9993,7 +9988,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="123" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E123"/>
       <c r="F123" s="6" t="s">
         <v>661</v>
@@ -10011,7 +10006,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="124" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E124"/>
       <c r="F124" s="6" t="s">
         <v>664</v>
@@ -10029,7 +10024,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="125" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E125"/>
       <c r="F125" s="6" t="s">
         <v>667</v>
@@ -10047,7 +10042,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="126" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E126"/>
       <c r="F126" s="6" t="s">
         <v>670</v>
@@ -10065,7 +10060,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E127"/>
       <c r="F127" s="6" t="s">
         <v>673</v>
@@ -10083,7 +10078,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="128" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E128"/>
       <c r="F128" s="6" t="s">
         <v>676</v>
@@ -10101,7 +10096,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E129"/>
       <c r="F129" s="6" t="s">
         <v>679</v>
@@ -10119,7 +10114,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="130" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E130"/>
       <c r="F130" s="6" t="s">
         <v>682</v>
@@ -10137,7 +10132,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="131" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E131"/>
       <c r="F131" s="6" t="s">
         <v>685</v>
@@ -10155,7 +10150,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="132" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E132"/>
       <c r="F132" s="6" t="s">
         <v>688</v>
@@ -10173,7 +10168,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="133" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E133"/>
       <c r="F133" s="6" t="s">
         <v>691</v>
@@ -10191,7 +10186,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="134" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E134"/>
       <c r="F134" s="6" t="s">
         <v>694</v>
@@ -10209,7 +10204,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="135" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E135"/>
       <c r="F135" s="6" t="s">
         <v>696</v>
@@ -10227,7 +10222,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="136" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E136"/>
       <c r="F136" s="6" t="s">
         <v>699</v>
@@ -10245,7 +10240,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="137" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E137"/>
       <c r="F137" s="6" t="s">
         <v>702</v>
@@ -10263,7 +10258,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="138" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E138"/>
       <c r="F138" s="6" t="s">
         <v>704</v>
@@ -10281,7 +10276,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="139" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E139"/>
       <c r="F139" s="6" t="s">
         <v>706</v>
@@ -10299,7 +10294,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="140" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E140"/>
       <c r="F140" s="6" t="s">
         <v>709</v>
@@ -10317,7 +10312,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="141" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E141"/>
       <c r="F141" s="6" t="s">
         <v>712</v>
@@ -10335,7 +10330,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="142" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E142"/>
       <c r="F142" s="6" t="s">
         <v>715</v>
@@ -10353,7 +10348,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="143" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E143"/>
       <c r="F143" s="6" t="s">
         <v>718</v>
@@ -10371,7 +10366,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="144" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E144"/>
       <c r="F144" s="6" t="s">
         <v>721</v>
@@ -10389,7 +10384,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="145" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E145"/>
       <c r="F145" s="6" t="s">
         <v>724</v>
@@ -10407,7 +10402,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="146" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E146"/>
       <c r="F146" s="6" t="s">
         <v>727</v>
@@ -10425,7 +10420,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="147" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E147"/>
       <c r="F147" s="6" t="s">
         <v>730</v>
@@ -10443,7 +10438,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="148" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E148"/>
       <c r="F148" s="6" t="s">
         <v>733</v>
@@ -10461,7 +10456,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="149" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E149"/>
       <c r="F149" s="6" t="s">
         <v>736</v>
@@ -10479,7 +10474,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="150" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="150" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E150"/>
       <c r="F150" s="6" t="s">
         <v>739</v>
@@ -10497,7 +10492,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="151" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E151"/>
       <c r="F151" s="6" t="s">
         <v>742</v>
@@ -10515,7 +10510,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="152" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="152" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E152"/>
       <c r="F152" s="6" t="s">
         <v>745</v>
@@ -10533,7 +10528,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="153" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="153" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E153"/>
       <c r="F153" s="6" t="s">
         <v>748</v>
@@ -10551,7 +10546,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="154" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="154" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E154"/>
       <c r="F154" s="6" t="s">
         <v>751</v>
@@ -10569,7 +10564,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="155" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="155" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E155"/>
       <c r="F155" s="6" t="s">
         <v>754</v>
@@ -10587,7 +10582,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="156" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="156" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E156"/>
       <c r="F156" s="6" t="s">
         <v>757</v>
@@ -10605,7 +10600,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="157" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="157" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E157"/>
       <c r="F157" s="6" t="s">
         <v>760</v>
@@ -10623,7 +10618,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="158" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E158"/>
       <c r="F158" s="6" t="s">
         <v>763</v>
@@ -10641,7 +10636,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="159" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="159" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E159"/>
       <c r="F159" s="6" t="s">
         <v>766</v>
@@ -10659,7 +10654,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="160" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E160"/>
       <c r="F160" s="6" t="s">
         <v>769</v>
@@ -10677,7 +10672,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="161" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="161" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E161"/>
       <c r="F161" s="6" t="s">
         <v>772</v>
@@ -10695,7 +10690,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="162" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="162" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E162"/>
       <c r="F162" s="6" t="s">
         <v>775</v>
@@ -10713,7 +10708,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="163" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="163" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E163"/>
       <c r="F163" s="6" t="s">
         <v>778</v>
@@ -10731,7 +10726,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="164" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="164" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E164"/>
       <c r="F164" s="6" t="s">
         <v>781</v>
@@ -10749,7 +10744,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="165" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="165" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E165"/>
       <c r="F165" s="6" t="s">
         <v>784</v>
@@ -10767,7 +10762,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="166" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="166" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E166"/>
       <c r="F166" s="6" t="s">
         <v>787</v>
@@ -10785,7 +10780,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="167" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="167" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E167"/>
       <c r="F167" s="6" t="s">
         <v>790</v>
@@ -10803,7 +10798,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="168" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="168" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E168"/>
       <c r="F168" s="6" t="s">
         <v>793</v>
@@ -10821,7 +10816,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="169" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="169" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E169"/>
       <c r="F169" s="6" t="s">
         <v>796</v>
@@ -10839,7 +10834,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="170" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="170" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E170"/>
       <c r="F170" s="6" t="s">
         <v>799</v>
@@ -10857,7 +10852,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="171" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="171" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E171"/>
       <c r="F171" s="6" t="s">
         <v>802</v>
@@ -10875,7 +10870,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="172" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="172" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E172"/>
       <c r="F172" s="6" t="s">
         <v>805</v>
@@ -10893,7 +10888,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="173" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="173" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E173"/>
       <c r="F173" s="6" t="s">
         <v>808</v>
@@ -10911,7 +10906,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="174" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="174" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E174"/>
       <c r="F174" s="6" t="s">
         <v>811</v>
@@ -10929,7 +10924,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="175" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="175" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E175"/>
       <c r="F175" s="6" t="s">
         <v>814</v>
@@ -10947,7 +10942,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="176" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="176" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E176"/>
       <c r="F176" s="6" t="s">
         <v>817</v>
@@ -10965,7 +10960,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="177" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E177"/>
       <c r="F177" s="6" t="s">
         <v>820</v>
@@ -10983,7 +10978,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="178" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="178" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E178"/>
       <c r="F178" s="6" t="s">
         <v>823</v>
@@ -11001,7 +10996,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="179" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E179"/>
       <c r="F179" s="6" t="s">
         <v>826</v>
@@ -11019,7 +11014,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="180" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E180"/>
       <c r="F180" s="6" t="s">
         <v>829</v>
@@ -11037,7 +11032,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="181" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E181"/>
       <c r="F181" s="6" t="s">
         <v>832</v>
@@ -11055,7 +11050,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="182" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="182" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E182"/>
       <c r="F182" s="6" t="s">
         <v>835</v>
@@ -11073,7 +11068,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="183" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="183" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E183"/>
       <c r="F183" s="6" t="s">
         <v>838</v>
@@ -11091,7 +11086,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="184" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="184" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E184"/>
       <c r="F184" s="6" t="s">
         <v>841</v>
@@ -11109,7 +11104,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="185" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="185" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E185"/>
       <c r="F185" s="6" t="s">
         <v>844</v>
@@ -11127,7 +11122,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="186" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="186" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E186"/>
       <c r="F186" s="6" t="s">
         <v>847</v>
@@ -11145,7 +11140,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="187" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="187" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E187"/>
       <c r="F187" s="6" t="s">
         <v>850</v>
@@ -11163,7 +11158,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="188" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="188" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E188"/>
       <c r="F188" s="6" t="s">
         <v>853</v>
@@ -11181,7 +11176,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="189" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="189" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E189"/>
       <c r="F189" s="6" t="s">
         <v>856</v>
@@ -11199,7 +11194,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="190" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="190" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E190"/>
       <c r="F190" s="6" t="s">
         <v>859</v>
@@ -11217,7 +11212,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="191" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="191" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E191"/>
       <c r="F191" s="6" t="s">
         <v>862</v>
@@ -11235,7 +11230,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="192" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="192" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E192"/>
       <c r="F192" s="6" t="s">
         <v>865</v>
@@ -11253,7 +11248,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="193" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="193" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E193"/>
       <c r="F193" s="6" t="s">
         <v>868</v>
@@ -11271,7 +11266,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="194" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="194" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E194"/>
       <c r="F194" s="6" t="s">
         <v>871</v>
@@ -11289,7 +11284,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="195" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="195" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E195"/>
       <c r="F195" s="6" t="s">
         <v>874</v>
@@ -11307,7 +11302,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="196" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="196" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E196"/>
       <c r="F196" s="6" t="s">
         <v>877</v>
@@ -11325,7 +11320,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="197" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="197" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E197"/>
       <c r="F197" s="6" t="s">
         <v>880</v>
@@ -11343,7 +11338,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="198" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="198" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E198"/>
       <c r="F198" s="6" t="s">
         <v>883</v>
@@ -11361,7 +11356,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="199" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="199" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E199"/>
       <c r="F199" s="6" t="s">
         <v>886</v>
@@ -11379,7 +11374,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="200" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E200"/>
       <c r="F200" s="6" t="s">
         <v>889</v>
@@ -11397,7 +11392,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="201" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E201"/>
       <c r="F201" s="6" t="s">
         <v>892</v>
@@ -11415,7 +11410,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="202" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E202"/>
       <c r="F202" s="6" t="s">
         <v>895</v>
@@ -11433,7 +11428,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="203" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E203"/>
       <c r="F203" s="6" t="s">
         <v>898</v>
@@ -11451,7 +11446,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="204" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E204"/>
       <c r="F204" s="6" t="s">
         <v>901</v>
@@ -11469,7 +11464,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="205" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E205"/>
       <c r="F205" s="6" t="s">
         <v>904</v>
@@ -11487,7 +11482,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="206" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="206" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E206"/>
       <c r="F206" s="6" t="s">
         <v>907</v>
@@ -11505,7 +11500,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="207" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="207" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E207"/>
       <c r="F207" s="6" t="s">
         <v>910</v>
@@ -11523,7 +11518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="208" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="208" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E208"/>
       <c r="F208" s="6" t="s">
         <v>912</v>
@@ -11541,7 +11536,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="209" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E209"/>
       <c r="F209" s="6" t="s">
         <v>915</v>
@@ -11559,7 +11554,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="210" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="210" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E210"/>
       <c r="F210" s="6" t="s">
         <v>918</v>
@@ -11577,7 +11572,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="211" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="211" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E211"/>
       <c r="F211" s="6" t="s">
         <v>921</v>
@@ -11595,7 +11590,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="212" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="212" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E212"/>
       <c r="F212" s="6" t="s">
         <v>924</v>
@@ -11613,7 +11608,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="213" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="213" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E213"/>
       <c r="F213" s="6" t="s">
         <v>927</v>
@@ -11631,7 +11626,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="214" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E214"/>
       <c r="F214" s="6" t="s">
         <v>930</v>
@@ -11649,7 +11644,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="215" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="215" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E215"/>
       <c r="F215" s="6" t="s">
         <v>933</v>
@@ -11667,7 +11662,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="216" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E216"/>
       <c r="F216" s="6" t="s">
         <v>936</v>
@@ -11685,7 +11680,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="217" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E217"/>
       <c r="F217" s="6" t="s">
         <v>939</v>
@@ -11703,7 +11698,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="218" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="218" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E218"/>
       <c r="F218" s="6" t="s">
         <v>942</v>
@@ -11721,7 +11716,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="219" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="219" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E219"/>
       <c r="F219" s="6" t="s">
         <v>945</v>
@@ -11739,7 +11734,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="220" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E220"/>
       <c r="F220" s="6" t="s">
         <v>948</v>
@@ -11757,7 +11752,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="221" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="221" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E221"/>
       <c r="F221" s="6" t="s">
         <v>951</v>
@@ -11775,7 +11770,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="222" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E222"/>
       <c r="F222" s="6" t="s">
         <v>954</v>
@@ -11793,7 +11788,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="223" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="223" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E223"/>
       <c r="F223" s="6" t="s">
         <v>957</v>
@@ -11811,7 +11806,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="224" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="224" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E224"/>
       <c r="F224" s="6" t="s">
         <v>960</v>
@@ -11829,7 +11824,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="225" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="225" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E225"/>
       <c r="F225" s="6" t="s">
         <v>963</v>
@@ -11859,15 +11854,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="10" max="10" width="126.33203125" customWidth="1"/>
+    <col min="10" max="10" width="126.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>199</v>
       </c>
@@ -11881,7 +11876,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -11893,7 +11888,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>200</v>
       </c>
@@ -11923,7 +11918,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="9" t="s">
         <v>207</v>
@@ -11951,7 +11946,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="9" t="s">
         <v>214</v>
@@ -11977,7 +11972,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
         <v>215</v>
@@ -12003,7 +11998,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
         <v>216</v>
@@ -12031,7 +12026,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
         <v>220</v>
@@ -12059,7 +12054,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="9" t="s">
         <v>221</v>
@@ -12087,7 +12082,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="9" t="s">
         <v>222</v>
@@ -12113,7 +12108,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
         <v>223</v>
@@ -12139,7 +12134,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="9" t="s">
         <v>224</v>
@@ -12165,7 +12160,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
         <v>225</v>
@@ -12193,7 +12188,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="9" t="s">
         <v>227</v>
@@ -12221,7 +12216,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
         <v>228</v>
@@ -12249,7 +12244,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -12263,7 +12258,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>229</v>
       </c>
@@ -12277,7 +12272,7 @@
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>230</v>
       </c>
@@ -12291,7 +12286,7 @@
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>200</v>
       </c>
@@ -12319,7 +12314,7 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>1</v>
       </c>
@@ -12349,7 +12344,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>2</v>
       </c>
@@ -12369,7 +12364,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>3</v>
       </c>
@@ -12384,7 +12379,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>4</v>
       </c>
@@ -12399,7 +12394,7 @@
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>5</v>
       </c>
@@ -12414,7 +12409,7 @@
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>6</v>
       </c>
@@ -12429,7 +12424,7 @@
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>7</v>
       </c>
@@ -12444,7 +12439,7 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>8</v>
       </c>
@@ -12459,7 +12454,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>9</v>
       </c>
@@ -12474,7 +12469,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>10</v>
       </c>
@@ -12489,7 +12484,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>11</v>
       </c>
@@ -12504,7 +12499,7 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>12</v>
       </c>
@@ -12519,7 +12514,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>13</v>
       </c>
@@ -12534,7 +12529,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>14</v>
       </c>
@@ -12549,7 +12544,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>15</v>
       </c>
@@ -12564,7 +12559,7 @@
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <v>16</v>
       </c>
@@ -12579,7 +12574,7 @@
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>17</v>
       </c>
@@ -12594,7 +12589,7 @@
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>18</v>
       </c>
@@ -12609,7 +12604,7 @@
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>19</v>
       </c>
@@ -12620,7 +12615,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>20</v>
       </c>
@@ -12631,7 +12626,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>21</v>
       </c>
@@ -12642,7 +12637,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>22</v>
       </c>
@@ -12653,7 +12648,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>23</v>
       </c>
@@ -12664,7 +12659,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>24</v>
       </c>
@@ -12675,7 +12670,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>25</v>
       </c>
@@ -12686,7 +12681,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>26</v>
       </c>
@@ -12697,7 +12692,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>27</v>
       </c>
@@ -12708,7 +12703,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>28</v>
       </c>
@@ -12719,7 +12714,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>29</v>
       </c>
@@ -12730,7 +12725,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>30</v>
       </c>
@@ -12741,7 +12736,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>31</v>
       </c>
@@ -12752,7 +12747,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>32</v>
       </c>
@@ -12763,7 +12758,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>33</v>
       </c>
@@ -12774,7 +12769,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>34</v>
       </c>
@@ -12785,7 +12780,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>35</v>
       </c>
@@ -12796,7 +12791,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>36</v>
       </c>
@@ -12807,7 +12802,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>37</v>
       </c>
@@ -12818,7 +12813,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>38</v>
       </c>
@@ -12829,7 +12824,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>39</v>
       </c>
@@ -12840,7 +12835,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>40</v>
       </c>
@@ -12851,7 +12846,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>41</v>
       </c>
@@ -12862,7 +12857,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>42</v>
       </c>
@@ -12873,7 +12868,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>43</v>
       </c>
@@ -12884,7 +12879,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>44</v>
       </c>
@@ -12895,7 +12890,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>45</v>
       </c>
@@ -12906,7 +12901,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>46</v>
       </c>
@@ -12917,7 +12912,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>47</v>
       </c>
@@ -12928,7 +12923,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>48</v>
       </c>
@@ -12939,7 +12934,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>49</v>
       </c>
@@ -12950,7 +12945,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>50</v>
       </c>
@@ -12961,7 +12956,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>51</v>
       </c>
@@ -12972,7 +12967,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>52</v>
       </c>
@@ -12983,7 +12978,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>53</v>
       </c>

</xml_diff>